<commit_message>
Fix #4007 Model SAM_MODEL.xlsx import error
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/SAM_MODEL.xlsx
+++ b/molgenis-model-registry/src/test/resources/SAM_MODEL.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="920" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="3285" yWindow="915" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="194">
   <si>
     <t>QNAME</t>
   </si>
@@ -604,6 +604,9 @@
   </si>
   <si>
     <t>SAM_TAG_Types</t>
+  </si>
+  <si>
+    <t>Regexp_</t>
   </si>
 </sst>
 </file>
@@ -787,6 +790,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1112,396 +1120,456 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="112.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="112.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>190</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="b">
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" t="b">
+      <c r="G2" t="b">
         <v>0</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>190</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="b">
+      <c r="G3" t="b">
         <v>0</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>190</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="b">
+      <c r="G4" t="b">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>190</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="b">
+      <c r="G5" t="b">
         <v>0</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>190</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="b">
+      <c r="G6" t="b">
         <v>0</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>190</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="b">
+      <c r="G7" t="b">
         <v>0</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
       <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
         <v>190</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" t="b">
+      <c r="G8" t="b">
         <v>0</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
         <v>190</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="F9" t="b">
+      <c r="G9" t="b">
         <v>0</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
         <v>190</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>30</v>
       </c>
-      <c r="F10" t="b">
+      <c r="G10" t="b">
         <v>0</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
         <v>190</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="F11" t="b">
+      <c r="G11" t="b">
         <v>0</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
         <v>190</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="F12" t="b">
+      <c r="G12" t="b">
         <v>0</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
         <v>190</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>135</v>
       </c>
       <c r="B14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" t="s">
         <v>190</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="E15" t="b">
+      <c r="F15" t="b">
         <v>1</v>
       </c>
-      <c r="F15" t="b">
+      <c r="G15" t="b">
         <v>0</v>
       </c>
-      <c r="O15" t="b">
+      <c r="P15" t="b">
         <v>1</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>107</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>192</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>110</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>29</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>109</v>
       </c>
       <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
         <v>192</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>32</v>
       </c>
-      <c r="E18" t="b">
+      <c r="F18" t="b">
         <v>1</v>
       </c>
-      <c r="F18" t="b">
+      <c r="G18" t="b">
         <v>0</v>
       </c>
-      <c r="J18" t="b">
+      <c r="K18" t="b">
         <v>1</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" t="s">
         <v>147</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>192</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>32</v>
       </c>
-      <c r="O19" t="b">
+      <c r="P19" t="b">
         <v>1</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>110</v>
       </c>
       <c r="B20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" t="s">
         <v>192</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>29</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1524,13 +1592,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1541,7 +1609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1552,7 +1620,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -1563,7 +1631,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -1593,13 +1661,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1613,7 +1681,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1643,12 +1711,12 @@
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1708,9 +1776,9 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>108</v>
       </c>
@@ -1721,7 +1789,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1732,7 +1800,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1743,7 +1811,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1754,7 +1822,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1765,7 +1833,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1776,7 +1844,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1787,7 +1855,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -1798,7 +1866,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -1809,7 +1877,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1820,7 +1888,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1831,7 +1899,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -1842,7 +1910,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -1853,7 +1921,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -1864,7 +1932,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1875,7 +1943,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -1886,7 +1954,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -1897,7 +1965,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -1908,7 +1976,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1919,7 +1987,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -1930,7 +1998,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -1941,7 +2009,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -1952,7 +2020,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -1963,7 +2031,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -1974,7 +2042,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -1985,7 +2053,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>102</v>
       </c>
@@ -1996,7 +2064,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2007,7 +2075,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -2018,7 +2086,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>113</v>
       </c>
@@ -2029,7 +2097,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>115</v>
       </c>
@@ -2040,7 +2108,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>117</v>
       </c>
@@ -2051,7 +2119,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -2062,7 +2130,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>121</v>
       </c>
@@ -2073,7 +2141,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>123</v>
       </c>
@@ -2084,7 +2152,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>125</v>
       </c>
@@ -2095,7 +2163,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>127</v>
       </c>
@@ -2106,7 +2174,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -2117,7 +2185,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -2128,7 +2196,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -2139,7 +2207,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>144</v>
       </c>
@@ -2150,7 +2218,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>136</v>
       </c>
@@ -2161,7 +2229,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>138</v>
       </c>
@@ -2172,7 +2240,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>140</v>
       </c>
@@ -2183,7 +2251,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>142</v>
       </c>
@@ -2210,23 +2278,23 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>109</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>193</v>
       </c>
       <c r="C1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -2237,7 +2305,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -2248,7 +2316,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>153</v>
       </c>
@@ -2259,7 +2327,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2270,7 +2338,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>158</v>
       </c>
@@ -2281,7 +2349,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -2310,16 +2378,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="41.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>173</v>
       </c>
@@ -2339,7 +2407,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>183</v>
       </c>
@@ -2359,7 +2427,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>184</v>
       </c>
@@ -2379,7 +2447,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>186</v>
       </c>

</xml_diff>